<commit_message>
Various changes - fixes from bug list - changes suggested in meetings
</commit_message>
<xml_diff>
--- a/Praescio/Template/StudentList.xlsx
+++ b/Praescio/Template/StudentList.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ali\Praescio 10 Jan\Praescio\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\avi\elysiar\pros\praescioedu\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{279E2E2A-486F-4657-97E4-F8B84C6C4976}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="12630"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TeacherList" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>FirstName</t>
   </si>
@@ -39,9 +41,6 @@
     <t>StudentMobileNo</t>
   </si>
   <si>
-    <t>Version</t>
-  </si>
-  <si>
     <t>Board</t>
   </si>
   <si>
@@ -63,21 +62,12 @@
     <t>ActivateOn</t>
   </si>
   <si>
-    <t>ExpiredOn</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>PinCode</t>
-  </si>
-  <si>
     <t>ALI</t>
   </si>
   <si>
@@ -90,9 +80,6 @@
     <t>ali.tech1108@gmail.com</t>
   </si>
   <si>
-    <t>PAID</t>
-  </si>
-  <si>
     <t>MH Board</t>
   </si>
   <si>
@@ -111,27 +98,76 @@
     <t>KURLA</t>
   </si>
   <si>
-    <t>MAHARASHTRA</t>
-  </si>
-  <si>
-    <t>MUMBAI</t>
+    <t>ASIF</t>
   </si>
   <si>
     <t>a</t>
   </si>
   <si>
-    <t>ASIF</t>
-  </si>
-  <si>
-    <t>24/10/2011</t>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>CBSE Board</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>ICSE Board</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>West Bengal</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
+    <numFmt numFmtId="165" formatCode="##########"/>
+  </numFmts>
+  <fonts count="4">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -166,15 +202,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -450,21 +488,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="14" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,220 +523,257 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="30">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="D2" s="4">
+        <v>31344</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="30">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="F2" s="5">
+        <v>7512323132</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" s="5">
+        <v>7512323132</v>
+      </c>
+      <c r="L2" s="4">
+        <v>31344</v>
+      </c>
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:13" ht="30">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4">
+        <v>31362</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5">
+        <v>7512323132</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="5">
+        <v>7512323132</v>
+      </c>
+      <c r="L3" s="4">
+        <v>31345</v>
+      </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4">
+        <v>31392</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5">
+        <v>7512323132</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="2">
-        <v>875</v>
-      </c>
-      <c r="O2" s="3">
-        <v>43108</v>
-      </c>
-      <c r="P2" s="3">
-        <v>43108</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2">
-        <v>400070</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="30">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="K4" s="5">
+        <v>7512323132</v>
+      </c>
+      <c r="L4" s="4">
+        <v>31346</v>
+      </c>
+      <c r="M4" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="2">
-        <v>875</v>
-      </c>
-      <c r="O3" s="3">
-        <v>43108</v>
-      </c>
-      <c r="P3" s="3">
-        <v>43108</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3">
-        <v>400070</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="30">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="2">
-        <v>875</v>
-      </c>
-      <c r="O4" s="3">
-        <v>43108</v>
-      </c>
-      <c r="P4" s="3">
-        <v>43108</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s">
-        <v>30</v>
-      </c>
-      <c r="S4" t="s">
-        <v>31</v>
-      </c>
-      <c r="T4">
-        <v>400070</v>
-      </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4" xr:uid="{1C7B3582-1003-4DDA-AC4F-26A80222E9C1}">
+      <formula1>"Male,Female"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 L2:L4" xr:uid="{05AD82F8-68DF-4B22-BA56-0EF2C5F31A2F}">
+      <formula1>D2&lt;TODAY()</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4 K2:K4" xr:uid="{1A343083-665A-4165-98F5-5CBEEAE483B3}">
+      <formula1>10</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
</xml_diff>